<commit_message>
AutoCommit_25 февраля 2024 г. 16:35:49_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-522_ТерВер.xlsx
+++ b/_2ИСИП-522_ТерВер.xlsx
@@ -501,10 +501,10 @@
   <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2:G2"/>
+      <selection pane="bottomRight" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -644,7 +644,9 @@
       <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="2"/>
+      <c r="C10" s="2">
+        <v>5</v>
+      </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -659,7 +661,9 @@
       <c r="B11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="2"/>
+      <c r="C11" s="2">
+        <v>5</v>
+      </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
@@ -719,7 +723,9 @@
       <c r="B15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="2"/>
+      <c r="C15" s="2">
+        <v>5</v>
+      </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
@@ -734,7 +740,9 @@
       <c r="B16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="2"/>
+      <c r="C16" s="2">
+        <v>5</v>
+      </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
@@ -779,7 +787,9 @@
       <c r="B19" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="2"/>
+      <c r="C19" s="2">
+        <v>5</v>
+      </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
@@ -794,7 +804,9 @@
       <c r="B20" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="2"/>
+      <c r="C20" s="2">
+        <v>5</v>
+      </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
@@ -809,7 +821,9 @@
       <c r="B21" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="2"/>
+      <c r="C21" s="2">
+        <v>5</v>
+      </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
@@ -839,7 +853,9 @@
       <c r="B23" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="2"/>
+      <c r="C23" s="2">
+        <v>5</v>
+      </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
@@ -869,7 +885,9 @@
       <c r="B25" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="2"/>
+      <c r="C25" s="2">
+        <v>5</v>
+      </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_1 марта 2024 г. 8:29:15_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-522_ТерВер.xlsx
+++ b/_2ИСИП-522_ТерВер.xlsx
@@ -504,7 +504,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C12" sqref="C12"/>
+      <selection pane="bottomRight" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -710,7 +710,9 @@
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
+      <c r="E14" s="2">
+        <v>5</v>
+      </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
@@ -727,7 +729,9 @@
         <v>5</v>
       </c>
       <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
+      <c r="E15" s="2">
+        <v>5</v>
+      </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_1 марта 2024 г. 10:03:40_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-522_ТерВер.xlsx
+++ b/_2ИСИП-522_ТерВер.xlsx
@@ -504,7 +504,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E15" sqref="E15"/>
+      <selection pane="bottomRight" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -647,8 +647,12 @@
       <c r="C10" s="2">
         <v>5</v>
       </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
+      <c r="D10" s="2">
+        <v>5</v>
+      </c>
+      <c r="E10" s="2">
+        <v>5</v>
+      </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
@@ -842,7 +846,9 @@
       <c r="B22" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="2"/>
+      <c r="C22" s="2">
+        <v>5</v>
+      </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
@@ -996,9 +1002,15 @@
       <c r="B32" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
+      <c r="C32" s="2">
+        <v>5</v>
+      </c>
+      <c r="D32" s="2">
+        <v>5</v>
+      </c>
+      <c r="E32" s="2">
+        <v>5</v>
+      </c>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_24 мая 2024 г. 10:03:33_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-522_ТерВер.xlsx
+++ b/_2ИСИП-522_ТерВер.xlsx
@@ -538,11 +538,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomRight" activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -573,8 +573,12 @@
       <c r="G2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
+      <c r="H2" s="1">
+        <v>6</v>
+      </c>
+      <c r="I2" s="1">
+        <v>7</v>
+      </c>
       <c r="J2" s="4" t="s">
         <v>35</v>
       </c>
@@ -812,11 +816,15 @@
       <c r="G10" s="2">
         <v>5</v>
       </c>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
+      <c r="H10" s="2">
+        <v>5</v>
+      </c>
+      <c r="I10" s="2">
+        <v>5</v>
+      </c>
       <c r="J10">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="K10">
         <v>5</v>

</xml_diff>

<commit_message>
AutoCommit_31 мая 2024 г. 8:31:44_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-522_ТерВер.xlsx
+++ b/_2ИСИП-522_ТерВер.xlsx
@@ -542,7 +542,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H10" sqref="H10"/>
+      <selection pane="bottomRight" activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1261,11 +1261,15 @@
       <c r="G23" s="2">
         <v>5</v>
       </c>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
+      <c r="H23" s="2">
+        <v>5</v>
+      </c>
+      <c r="I23" s="2">
+        <v>5</v>
+      </c>
       <c r="J23">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="K23">
         <v>5</v>

</xml_diff>

<commit_message>
AutoCommit_31 мая 2024 г. 9:40:21_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-522_ТерВер.xlsx
+++ b/_2ИСИП-522_ТерВер.xlsx
@@ -542,7 +542,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J23" sqref="J23"/>
+      <selection pane="bottomRight" activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -886,11 +886,11 @@
         <v>5</v>
       </c>
       <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12">
-        <f t="shared" si="0"/>
-        <v>20</v>
+      <c r="H12" s="2">
+        <v>5</v>
+      </c>
+      <c r="I12" s="2">
+        <v>5</v>
       </c>
       <c r="K12">
         <v>5</v>
@@ -1080,13 +1080,13 @@
         <v>15</v>
       </c>
       <c r="C18" s="5">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D18" s="5">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E18" s="5">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F18" s="5">
         <v>2</v>
@@ -1096,7 +1096,7 @@
       <c r="I18" s="2"/>
       <c r="J18">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="K18">
         <v>3</v>
@@ -1159,12 +1159,14 @@
       <c r="F20" s="2">
         <v>5</v>
       </c>
-      <c r="G20" s="2"/>
+      <c r="G20" s="2">
+        <v>5</v>
+      </c>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="K20">
         <v>4</v>
@@ -1192,12 +1194,14 @@
       <c r="F21" s="2">
         <v>5</v>
       </c>
-      <c r="G21" s="2"/>
+      <c r="G21" s="2">
+        <v>5</v>
+      </c>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="K21">
         <v>3</v>
@@ -1225,12 +1229,14 @@
       <c r="F22" s="2">
         <v>5</v>
       </c>
-      <c r="G22" s="2"/>
+      <c r="G22" s="2">
+        <v>5</v>
+      </c>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="K22">
         <v>4</v>

</xml_diff>

<commit_message>
AutoCommit_7 июня 2024 г. 9:40:42_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-522_ТерВер.xlsx
+++ b/_2ИСИП-522_ТерВер.xlsx
@@ -539,10 +539,10 @@
   <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F18" sqref="F18"/>
+      <selection pane="bottomRight" activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -713,11 +713,15 @@
         <v>2</v>
       </c>
       <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
+      <c r="H7" s="2">
+        <v>5</v>
+      </c>
+      <c r="I7" s="2">
+        <v>5</v>
+      </c>
       <c r="J7">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="K7">
         <v>4</v>
@@ -885,7 +889,9 @@
       <c r="F12" s="5">
         <v>5</v>
       </c>
-      <c r="G12" s="2"/>
+      <c r="G12" s="2">
+        <v>5</v>
+      </c>
       <c r="H12" s="2">
         <v>5</v>
       </c>
@@ -1473,11 +1479,13 @@
       <c r="G29" s="2">
         <v>5</v>
       </c>
-      <c r="H29" s="2"/>
+      <c r="H29" s="2">
+        <v>5</v>
+      </c>
       <c r="I29" s="2"/>
       <c r="J29">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="K29">
         <v>3</v>

</xml_diff>

<commit_message>
AutoCommit_14 июня 2024 г. 11:24:15_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-522_ТерВер.xlsx
+++ b/_2ИСИП-522_ТерВер.xlsx
@@ -171,7 +171,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -205,11 +205,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -230,6 +239,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -542,7 +554,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J12" sqref="J12"/>
+      <selection pane="bottomRight" activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -987,9 +999,12 @@
       <c r="I16" s="2">
         <v>5</v>
       </c>
+      <c r="J16" s="7">
+        <v>5</v>
+      </c>
       <c r="K16">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="13" x14ac:dyDescent="0.25">
@@ -1185,9 +1200,12 @@
       <c r="I22" s="2">
         <v>5</v>
       </c>
+      <c r="J22" s="7">
+        <v>5</v>
+      </c>
       <c r="K22">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="13" x14ac:dyDescent="0.25">
@@ -1218,9 +1236,12 @@
       <c r="I23" s="2">
         <v>5</v>
       </c>
+      <c r="J23" s="8">
+        <v>5</v>
+      </c>
       <c r="K23">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
AutoCommit_14 июня 2024 г. 11:26:40_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-522_ТерВер.xlsx
+++ b/_2ИСИП-522_ТерВер.xlsx
@@ -551,10 +551,10 @@
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J23" sqref="J23"/>
+      <selection pane="bottomRight" activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1374,11 +1374,15 @@
       <c r="G28" s="2">
         <v>5</v>
       </c>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
+      <c r="H28" s="2">
+        <v>5</v>
+      </c>
+      <c r="I28" s="2">
+        <v>5</v>
+      </c>
       <c r="K28">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
AutoCommit_14 июня 2024 г. 11:28:22_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-522_ТерВер.xlsx
+++ b/_2ИСИП-522_ТерВер.xlsx
@@ -551,10 +551,10 @@
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J28" sqref="J28"/>
+      <selection pane="bottomRight" activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -937,9 +937,12 @@
       <c r="I14" s="2">
         <v>5</v>
       </c>
+      <c r="J14" s="7">
+        <v>5</v>
+      </c>
       <c r="K14">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
AutoCommit_15 июня 2024 г. 14:19:01_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-522_ТерВер.xlsx
+++ b/_2ИСИП-522_ТерВер.xlsx
@@ -557,7 +557,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="N28" sqref="N28"/>
+      <selection pane="bottomRight" activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1494,16 +1494,16 @@
         <v>28</v>
       </c>
       <c r="C31" s="5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D31" s="5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E31" s="5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F31" s="5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G31" s="2">
         <v>5</v>
@@ -1516,7 +1516,7 @@
       </c>
       <c r="K31">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="32" spans="1:14" ht="13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
AutoCommit_15 июня 2024 г. 22:37:40_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-522_ТерВер.xlsx
+++ b/_2ИСИП-522_ТерВер.xlsx
@@ -554,10 +554,10 @@
   <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G31" sqref="G31"/>
+      <selection pane="bottomRight" activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -600,13 +600,30 @@
       <c r="K2" s="4"/>
     </row>
     <row r="3" spans="1:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1">
+        <v>1</v>
+      </c>
+      <c r="I3" s="1">
+        <v>1</v>
+      </c>
+      <c r="J3" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
@@ -699,12 +716,21 @@
       <c r="F6" s="5">
         <v>2</v>
       </c>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
+      <c r="G6" s="2">
+        <v>2</v>
+      </c>
+      <c r="H6" s="2">
+        <v>2</v>
+      </c>
+      <c r="I6" s="2">
+        <v>2</v>
+      </c>
+      <c r="J6" s="7">
+        <v>2</v>
+      </c>
       <c r="K6">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="13" x14ac:dyDescent="0.25">
@@ -735,9 +761,12 @@
       <c r="I7" s="2">
         <v>5</v>
       </c>
+      <c r="J7" s="8">
+        <v>2</v>
+      </c>
       <c r="K7">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="13" x14ac:dyDescent="0.25">
@@ -762,11 +791,18 @@
       <c r="G8" s="2">
         <v>5</v>
       </c>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
+      <c r="H8" s="2">
+        <v>2</v>
+      </c>
+      <c r="I8" s="2">
+        <v>2</v>
+      </c>
+      <c r="J8" s="8">
+        <v>2</v>
+      </c>
       <c r="K8">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="13" x14ac:dyDescent="0.25">
@@ -788,12 +824,21 @@
       <c r="F9" s="2">
         <v>5</v>
       </c>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
+      <c r="G9" s="2">
+        <v>2</v>
+      </c>
+      <c r="H9" s="2">
+        <v>2</v>
+      </c>
+      <c r="I9" s="2">
+        <v>2</v>
+      </c>
+      <c r="J9" s="8">
+        <v>2</v>
+      </c>
       <c r="K9">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="13" x14ac:dyDescent="0.25">
@@ -824,9 +869,12 @@
       <c r="I10" s="2">
         <v>5</v>
       </c>
+      <c r="J10" s="8">
+        <v>2</v>
+      </c>
       <c r="K10">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="13" x14ac:dyDescent="0.25">
@@ -857,9 +905,12 @@
       <c r="I11" s="2">
         <v>5</v>
       </c>
+      <c r="J11" s="8">
+        <v>2</v>
+      </c>
       <c r="K11">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="13" x14ac:dyDescent="0.25">
@@ -920,11 +971,18 @@
       <c r="G13" s="2">
         <v>5</v>
       </c>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
+      <c r="H13" s="2">
+        <v>2</v>
+      </c>
+      <c r="I13" s="2">
+        <v>2</v>
+      </c>
+      <c r="J13" s="8">
+        <v>2</v>
+      </c>
       <c r="K13">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="13" x14ac:dyDescent="0.25">
@@ -1054,12 +1112,21 @@
       <c r="F17" s="5">
         <v>2</v>
       </c>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
+      <c r="G17" s="2">
+        <v>2</v>
+      </c>
+      <c r="H17" s="2">
+        <v>2</v>
+      </c>
+      <c r="I17" s="2">
+        <v>2</v>
+      </c>
+      <c r="J17" s="8">
+        <v>2</v>
+      </c>
       <c r="K17">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="13" x14ac:dyDescent="0.25">
@@ -1198,9 +1265,12 @@
       <c r="I21" s="2">
         <v>5</v>
       </c>
+      <c r="J21" s="8">
+        <v>2</v>
+      </c>
       <c r="K21">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="13" x14ac:dyDescent="0.25">
@@ -1294,12 +1364,21 @@
       <c r="F24" s="5">
         <v>5</v>
       </c>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
+      <c r="G24" s="2">
+        <v>2</v>
+      </c>
+      <c r="H24" s="2">
+        <v>2</v>
+      </c>
+      <c r="I24" s="2">
+        <v>2</v>
+      </c>
+      <c r="J24" s="8">
+        <v>2</v>
+      </c>
       <c r="K24">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="13" x14ac:dyDescent="0.25">
@@ -1321,12 +1400,21 @@
       <c r="F25" s="5">
         <v>2</v>
       </c>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
+      <c r="G25" s="2">
+        <v>2</v>
+      </c>
+      <c r="H25" s="2">
+        <v>2</v>
+      </c>
+      <c r="I25" s="2">
+        <v>2</v>
+      </c>
+      <c r="J25" s="8">
+        <v>2</v>
+      </c>
       <c r="K25">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="13" x14ac:dyDescent="0.25">
@@ -1351,7 +1439,9 @@
       <c r="G26" s="2">
         <v>5</v>
       </c>
-      <c r="H26" s="2"/>
+      <c r="H26" s="2">
+        <v>2</v>
+      </c>
       <c r="I26" s="2">
         <v>5</v>
       </c>
@@ -1360,7 +1450,7 @@
       </c>
       <c r="K26">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="N26" t="s">
         <v>36</v>
@@ -1385,12 +1475,21 @@
       <c r="F27" s="5">
         <v>5</v>
       </c>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
+      <c r="G27" s="2">
+        <v>2</v>
+      </c>
+      <c r="H27" s="2">
+        <v>2</v>
+      </c>
+      <c r="I27" s="2">
+        <v>2</v>
+      </c>
+      <c r="J27" s="8">
+        <v>2</v>
+      </c>
       <c r="K27">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>28</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="13" x14ac:dyDescent="0.25">
@@ -1421,9 +1520,12 @@
       <c r="I28" s="2">
         <v>5</v>
       </c>
+      <c r="J28" s="8">
+        <v>2</v>
+      </c>
       <c r="K28">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="13" x14ac:dyDescent="0.25">
@@ -1451,10 +1553,15 @@
       <c r="H29" s="2">
         <v>5</v>
       </c>
-      <c r="I29" s="2"/>
+      <c r="I29" s="2">
+        <v>2</v>
+      </c>
+      <c r="J29" s="8">
+        <v>2</v>
+      </c>
       <c r="K29">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="13" x14ac:dyDescent="0.25">
@@ -1479,11 +1586,18 @@
       <c r="G30" s="2">
         <v>5</v>
       </c>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
+      <c r="H30" s="2">
+        <v>2</v>
+      </c>
+      <c r="I30" s="2">
+        <v>2</v>
+      </c>
+      <c r="J30" s="8">
+        <v>2</v>
+      </c>
       <c r="K30">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>31</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="13" x14ac:dyDescent="0.25">
@@ -1514,9 +1628,12 @@
       <c r="I31" s="2">
         <v>5</v>
       </c>
+      <c r="J31" s="8">
+        <v>2</v>
+      </c>
       <c r="K31">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="32" spans="1:14" ht="13" x14ac:dyDescent="0.25">
@@ -1541,11 +1658,18 @@
       <c r="G32" s="2">
         <v>5</v>
       </c>
-      <c r="H32" s="2"/>
-      <c r="I32" s="2"/>
+      <c r="H32" s="2">
+        <v>2</v>
+      </c>
+      <c r="I32" s="2">
+        <v>2</v>
+      </c>
+      <c r="J32" s="8">
+        <v>2</v>
+      </c>
       <c r="K32">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>31</v>
       </c>
     </row>
     <row r="33" spans="3:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
AutoCommit_16 июня 2024 г. 12:32:27_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-522_ТерВер.xlsx
+++ b/_2ИСИП-522_ТерВер.xlsx
@@ -546,10 +546,10 @@
   <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="M35" sqref="M35"/>
+      <selection pane="bottomRight" activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -805,11 +805,11 @@
         <v>0</v>
       </c>
       <c r="J8" s="6">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L8">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="M8">
         <v>4</v>

</xml_diff>

<commit_message>
AutoCommit_16 июня 2024 г. 13:23:29_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-522_ТерВер.xlsx
+++ b/_2ИСИП-522_ТерВер.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>2ИСИП-522: Теория вероятностей и математическая статистика (Сибирев И. В.) - II семестр</t>
   </si>
@@ -133,6 +133,9 @@
   </si>
   <si>
     <t>Сумма</t>
+  </si>
+  <si>
+    <t>ИЗМ</t>
   </si>
 </sst>
 </file>
@@ -543,13 +546,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N33"/>
+  <dimension ref="A1:O33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J8" sqref="J8"/>
+      <selection pane="bottomRight" activeCell="O31" sqref="O31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1127,7 +1130,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" ht="13" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>14</v>
       </c>
@@ -1166,7 +1169,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" ht="13" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>15</v>
       </c>
@@ -1205,7 +1208,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" ht="13" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>16</v>
       </c>
@@ -1244,7 +1247,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" ht="13" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>17</v>
       </c>
@@ -1283,7 +1286,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" ht="13" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>18</v>
       </c>
@@ -1322,7 +1325,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" ht="13" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>19</v>
       </c>
@@ -1361,7 +1364,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" ht="13" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>20</v>
       </c>
@@ -1400,7 +1403,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" ht="13" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>21</v>
       </c>
@@ -1439,7 +1442,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" ht="13" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>22</v>
       </c>
@@ -1478,7 +1481,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" ht="13" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>23</v>
       </c>
@@ -1520,7 +1523,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" ht="13" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>24</v>
       </c>
@@ -1559,7 +1562,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" ht="13" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>25</v>
       </c>
@@ -1598,7 +1601,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" ht="13" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>26</v>
       </c>
@@ -1637,7 +1640,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" ht="13" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>27</v>
       </c>
@@ -1660,23 +1663,26 @@
         <v>5</v>
       </c>
       <c r="H30" s="4">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I30" s="4">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J30" s="6">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L30">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="M30">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" ht="13" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="O30" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" ht="13" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>28</v>
       </c>
@@ -1715,7 +1721,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" ht="13" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>29</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_16 июня 2024 г. 16:56:36_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-522_ТерВер.xlsx
+++ b/_2ИСИП-522_ТерВер.xlsx
@@ -135,7 +135,7 @@
     <t>Сумма</t>
   </si>
   <si>
-    <t>ИЗМ</t>
+    <t>изм</t>
   </si>
 </sst>
 </file>
@@ -551,13 +551,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O33"/>
+  <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="M33" sqref="M33"/>
+      <selection pane="bottomRight" activeCell="C33" sqref="C33:M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -603,30 +603,14 @@
       </c>
     </row>
     <row r="3" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="1">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1">
-        <v>1</v>
-      </c>
-      <c r="E3" s="1">
-        <v>1</v>
-      </c>
-      <c r="F3" s="1">
-        <v>1</v>
-      </c>
-      <c r="G3" s="1">
-        <v>1</v>
-      </c>
-      <c r="H3" s="1">
-        <v>1</v>
-      </c>
-      <c r="I3" s="1">
-        <v>1</v>
-      </c>
-      <c r="J3" s="2">
-        <v>1</v>
-      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="2"/>
     </row>
     <row r="4" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
@@ -1136,7 +1120,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" ht="13" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>14</v>
       </c>
@@ -1175,7 +1159,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" ht="13" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>15</v>
       </c>
@@ -1214,7 +1198,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" ht="13" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>16</v>
       </c>
@@ -1253,7 +1237,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" ht="13" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>17</v>
       </c>
@@ -1292,7 +1276,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" ht="13" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>18</v>
       </c>
@@ -1331,7 +1315,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" ht="13" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>19</v>
       </c>
@@ -1370,7 +1354,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" ht="13" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>20</v>
       </c>
@@ -1409,7 +1393,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" ht="13" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>21</v>
       </c>
@@ -1448,7 +1432,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" ht="13" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>22</v>
       </c>
@@ -1487,7 +1471,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" ht="13" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>23</v>
       </c>
@@ -1529,7 +1513,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" ht="13" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>24</v>
       </c>
@@ -1568,7 +1552,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" ht="13" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>25</v>
       </c>
@@ -1607,7 +1591,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" ht="13" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>26</v>
       </c>
@@ -1646,7 +1630,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" ht="13" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>27</v>
       </c>
@@ -1684,11 +1668,8 @@
       <c r="M30">
         <v>5</v>
       </c>
-      <c r="O30" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:14" ht="13" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>28</v>
       </c>
@@ -1727,7 +1708,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" ht="13" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>29</v>
       </c>
@@ -1750,51 +1731,34 @@
         <v>5</v>
       </c>
       <c r="H32" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I32" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J32" s="5">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="L32">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="M32">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C33" s="8">
-        <v>1</v>
-      </c>
-      <c r="D33" s="8">
-        <v>1</v>
-      </c>
-      <c r="E33" s="8">
-        <v>1</v>
-      </c>
-      <c r="F33" s="8">
-        <v>1</v>
-      </c>
-      <c r="G33" s="8">
-        <v>1</v>
-      </c>
-      <c r="H33" s="8">
-        <v>1</v>
-      </c>
-      <c r="I33" s="8">
-        <v>1</v>
-      </c>
-      <c r="J33" s="9">
-        <v>1</v>
-      </c>
-      <c r="L33">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="N32" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="33" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="8"/>
+      <c r="J33" s="9"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>

</xml_diff>